<commit_message>
v2 of (se corrigieron bugs) DB: Se quitaron campos sin uso en tabla req_registro DB: Se quito campo persona sin uso en tabla requisitos Se modifico el metodo que carga el filtro para seleccion de persona en base al dpto del workflow Se inicio el metodo para impresion de reportes
</commit_message>
<xml_diff>
--- a/archivos/04 - Querys Insert registro, estado_actual_flujo/Datos registro, estado_actual_flujo.xlsx
+++ b/archivos/04 - Querys Insert registro, estado_actual_flujo/Datos registro, estado_actual_flujo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1" windowWidth="15090" windowHeight="6510"/>
+    <workbookView activeTab="3" windowWidth="15090" windowHeight="6510"/>
   </bookViews>
   <sheets>
     <sheet name="Registro" sheetId="1" r:id="rId1"/>
@@ -93,40 +93,40 @@
     <t>id_dest</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden, persona) values (</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden, persona) values (1,1,2,4,'Foto',TRUE,1,TRUE);</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden, persona) values (2,1,2,4,'Antecedentes policiales',TRUE,2,FALSE);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden, persona) values (3,1,2,4,'Una manzana',TRUE,3,FALSE);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (11,1,1,2,4,NULL,NULL,TRUE,4);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (11,2,1,2,4,NULL,NULL,TRUE,NULL);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (11,3,1,2,4,NULL,NULL,TRUE,NULL);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (14,1,1,2,4,NULL,NULL,TRUE,1);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (14,2,1,2,4,NULL,NULL,TRUE,NULL);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.requisitos_registro(id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, observacion, archivo, completo, id_persona) values (14,3,1,2,4,NULL,NULL,TRUE,NULL);</t>
+    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden) values (</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden) values (1,1,2,4,'Foto',TRUE,1);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden) values (2,1,2,4,'Antecedentes policiales',TRUE,2);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden) values (3,1,2,4,'Una manzana',TRUE,3);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos(id_requisitos, id_estadoorigen, id_estadodestino, id_workflow, nombre, obligatorio, orden) values (4,2,4,4,'Fecha vigencia',FALSE,1);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (1,1,1,1,2,4,NULL,TRUE);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (2,1,2,1,2,4,NULL,TRUE);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (3,1,3,1,2,4,NULL,TRUE);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (4,3,1,1,2,4,NULL,TRUE);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (5,3,2,1,2,4,NULL,TRUE);</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.requisitos_registro(id_requisitos_registro, id_registro, id_requisitos, id_estadoorigen, id_estadodestino, id_workflow,  archivo, completo) values (6,3,3,1,2,4,NULL,TRUE);</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="75">
       <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
@@ -583,10 +583,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N4"/>
+      <selection activeCell="N2" sqref="N2:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -622,11 +622,7 @@
           <t>orden</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>persona</t>
-        </is>
-      </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
@@ -652,15 +648,12 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
       <c r="J2" t="s">
         <v>21</v>
       </c>
       <c r="K2" t="str">
-        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;")"</f>
-        <v>1,1,2,4,'Foto',TRUE,1,TRUE)</v>
+        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;F2&amp;","&amp;G2&amp;")"</f>
+        <v>1,1,2,4,'Foto',TRUE,1)</v>
       </c>
       <c r="M2" t="s">
         <f>J2&amp;K2&amp;";"</f>
@@ -694,22 +687,19 @@
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
       <c r="J3" t="s">
         <v>21</v>
       </c>
       <c r="K3" t="str">
-        <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;")"</f>
-        <v>2,1,2,4,'Antecedentes policiales',TRUE,2,FALSE)</v>
+        <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;F3&amp;","&amp;G3&amp;")"</f>
+        <v>2,1,2,4,'Antecedentes policiales',TRUE,2)</v>
       </c>
       <c r="M3" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -736,21 +726,59 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
       <c r="K4" t="str">
-        <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;")"</f>
-        <v>3,1,2,4,'Una manzana',TRUE,3,FALSE)</v>
+        <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;F4&amp;","&amp;G4&amp;")"</f>
+        <v>3,1,2,4,'Una manzana',TRUE,3)</v>
       </c>
       <c r="M4" t="s">
         <f>J4&amp;K4&amp;";"</f>
+        <v>24</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Fecha vigencia</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="str">
+        <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;"'"&amp;E5&amp;"'"&amp;","&amp;F5&amp;","&amp;G5&amp;")"</f>
+        <v>4,2,4,4,'Fecha vigencia',FALSE,1)</v>
+      </c>
+      <c r="M5" t="s">
+        <f>J5&amp;K5&amp;";"</f>
         <v>25</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -771,310 +799,293 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="11" style="0" width="9.142307692307693"/>
-    <col min="12" max="12" style="0" width="28.141165865384618" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" style="0" width="9.142307692307693"/>
+    <col min="1" max="12" style="0" width="9.142307692307693"/>
+    <col min="13" max="13" style="0" width="28.141165865384618" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id_req_reg</t>
+        </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>id_reg</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>id_req</t>
         </is>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>completo</t>
+        </is>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="str">
+        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;H2&amp;","&amp;I2&amp;")"</f>
+        <v>1,1,1,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O2" t="s">
+        <f>L2&amp;M2&amp;";"</f>
+        <v>27</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="str">
+        <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;H3&amp;","&amp;I3&amp;")"</f>
+        <v>2,1,2,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O3" t="s">
+        <f>L3&amp;M3&amp;";"</f>
+        <v>28</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>completo</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>id_persona</t>
-        </is>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="str">
-        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;")"</f>
-        <v>11,1,1,2,4,NULL,NULL,TRUE,4)</v>
-      </c>
-      <c r="N2" t="s">
-        <f>K2&amp;L2&amp;";"</f>
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="M4" t="str">
+        <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;H4&amp;","&amp;I4&amp;")"</f>
+        <v>3,1,3,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O4" t="s">
+        <f>L4&amp;M4&amp;";"</f>
+        <v>29</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="str">
-        <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;")"</f>
-        <v>11,2,1,2,4,NULL,NULL,TRUE,NULL)</v>
-      </c>
-      <c r="N3" t="s">
-        <f>K3&amp;L3&amp;";"</f>
-        <v>28</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
+      <c r="M5" t="str">
+        <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;H5&amp;","&amp;I5&amp;")"</f>
+        <v>4,3,1,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O5" t="s">
+        <f>L5&amp;M5&amp;";"</f>
+        <v>30</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="str">
-        <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4&amp;")"</f>
-        <v>11,3,1,2,4,NULL,NULL,TRUE,NULL)</v>
-      </c>
-      <c r="N4" t="s">
-        <f>K4&amp;L4&amp;";"</f>
-        <v>29</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="str">
-        <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;")"</f>
-        <v>14,1,1,2,4,NULL,NULL,TRUE,1)</v>
-      </c>
-      <c r="N5" t="s">
-        <f>K5&amp;L5&amp;";"</f>
-        <v>30</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="str">
-        <f>A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6&amp;")"</f>
-        <v>14,2,1,2,4,NULL,NULL,TRUE,NULL)</v>
-      </c>
-      <c r="N6" t="s">
-        <f>K6&amp;L6&amp;";"</f>
+      <c r="M6" t="str">
+        <f>A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;","&amp;H6&amp;","&amp;I6&amp;")"</f>
+        <v>5,3,2,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O6" t="s">
+        <f>L6&amp;M6&amp;";"</f>
         <v>31</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="str">
-        <f>A7&amp;","&amp;B7&amp;","&amp;C7&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;")"</f>
-        <v>14,3,1,2,4,NULL,NULL,TRUE,NULL)</v>
-      </c>
-      <c r="N7" t="s">
-        <f>K7&amp;L7&amp;";"</f>
+      <c r="M7" t="str">
+        <f>A7&amp;","&amp;B7&amp;","&amp;C7&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;H7&amp;","&amp;I7&amp;")"</f>
+        <v>6,3,3,1,2,4,NULL,TRUE)</v>
+      </c>
+      <c r="O7" t="s">
+        <f>L7&amp;M7&amp;";"</f>
         <v>32</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementacion OK -Modif tabla registro y estado_actual (get_usuario) -Modif de modulos que usan los campos alterados Reporte: Finalizado reportes Detalle registros (error subreporte)
Pendiente
Inconvenientes con la creacion del email por modif de
empleados. Se debe trabajar el if que arma la resp ocultando/mostrando
la tabla detalle de los valores modificados.
</commit_message>
<xml_diff>
--- a/archivos/04 - Querys Insert registro, estado_actual_flujo/Datos registro, estado_actual_flujo.xlsx
+++ b/archivos/04 - Querys Insert registro, estado_actual_flujo/Datos registro, estado_actual_flujo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="3" windowWidth="15090" windowHeight="6510"/>
+    <workbookView activeTab="1" windowWidth="15090" windowHeight="6510"/>
   </bookViews>
   <sheets>
     <sheet name="Registro" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32" count="32">
   <si>
     <t>ID</t>
   </si>
@@ -39,9 +39,6 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>obs</t>
-  </si>
-  <si>
     <t>archivo</t>
   </si>
   <si>
@@ -75,16 +72,16 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado) values (</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado) values (1,'2017-09-09 14:29:08.308049'::TIMESTAMP,'TRUE',11,2);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado) values (2,'2017-09-09 16:38:03.599437'::TIMESTAMP,'TRUE',12,2);</t>
-  </si>
-  <si>
-    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado) values (3,'2017-09-30 09:37:15.278727'::TIMESTAMP,'TRUE',14,2);</t>
+    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado, get_usuario) values (</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado, get_usuario) values (1,'2017-09-09 14:29:08.308049'::TIMESTAMP,'TRUE',11,2,'toba');</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado, get_usuario) values (2,'2017-09-09 16:38:03.599437'::TIMESTAMP,'TRUE',12,2,'toba');</t>
+  </si>
+  <si>
+    <t>INSERT INTO sgr.estado_actual_flujo(id_estado_actual, fecha, activo, id_registro, id_estado, get_usuario) values (3,'2017-09-30 09:37:15.278727'::TIMESTAMP,'TRUE',14,2,'toba');</t>
   </si>
   <si>
     <t>id_orig</t>
@@ -250,11 +247,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>obs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
@@ -290,19 +289,19 @@
         </is>
       </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
       <c r="K2" t="str">
         <f>A2&amp;","&amp;B2&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;"'"&amp;D2&amp;"'"&amp;","&amp;E2&amp;","&amp;"'"&amp;F2&amp;"'"&amp;","&amp;"'"&amp;G2&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;H2&amp;")"</f>
@@ -310,10 +309,10 @@
       </c>
       <c r="M2" t="s">
         <f>J2&amp;K2&amp;";"</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -334,19 +333,19 @@
         </is>
       </c>
       <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K3" t="str">
         <f>A3&amp;","&amp;B3&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;"'"&amp;D3&amp;"'"&amp;","&amp;E3&amp;","&amp;"'"&amp;F3&amp;"'"&amp;","&amp;"'"&amp;G3&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;H3&amp;")"</f>
@@ -354,10 +353,10 @@
       </c>
       <c r="M3" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -378,19 +377,19 @@
         </is>
       </c>
       <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" t="str">
         <f>A4&amp;","&amp;B4&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;"'"&amp;D4&amp;"'"&amp;","&amp;E4&amp;","&amp;"'"&amp;F4&amp;"'"&amp;","&amp;"'"&amp;G4&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;H4&amp;")"</f>
@@ -398,10 +397,10 @@
       </c>
       <c r="M4" t="s">
         <f>J4&amp;K4&amp;";"</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -421,22 +420,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75">
-      <selection activeCell="K2" sqref="K2:K4"/>
+    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="9.142307692307693"/>
     <col min="2" max="2" style="0" width="27.28407451923077" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" style="0" width="9.142307692307693"/>
-    <col min="8" max="8" style="0" width="57.13942307692308" customWidth="1"/>
-    <col min="9" max="16384" style="0" width="9.142307692307693"/>
+    <col min="3" max="8" style="0" width="9.142307692307693"/>
+    <col min="9" max="9" style="0" width="57.13942307692308" customWidth="1"/>
+    <col min="10" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,16 +459,21 @@
           <t>id_estado</t>
         </is>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>get_usr</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -477,30 +481,33 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="str">
+        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;"'"&amp;F2&amp;"'"&amp;")"</f>
+        <v>1,'2017-09-09 14:29:08.308049'::TIMESTAMP,'TRUE',11,2,'toba')</v>
+      </c>
+      <c r="K2" t="s">
+        <f>H2&amp;I2&amp;";"</f>
         <v>15</v>
       </c>
-      <c r="H2" t="str">
-        <f>A2&amp;","&amp;"'"&amp;B2&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C2&amp;"'"&amp;","&amp;D2&amp;","&amp;E2&amp;")"</f>
-        <v>1,'2017-09-09 14:29:08.308049'::TIMESTAMP,'TRUE',11,2)</v>
-      </c>
-      <c r="J2" t="s">
-        <f>G2&amp;H2&amp;";"</f>
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>12</v>
@@ -508,30 +515,33 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="str">
-        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;D3&amp;","&amp;E3&amp;")"</f>
-        <v>2,'2017-09-09 16:38:03.599437'::TIMESTAMP,'TRUE',12,2)</v>
-      </c>
-      <c r="J3" t="s">
-        <f>G3&amp;H3&amp;";"</f>
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="str">
+        <f>A3&amp;","&amp;"'"&amp;B3&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C3&amp;"'"&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;"'"&amp;F3&amp;"'"&amp;")"</f>
+        <v>2,'2017-09-09 16:38:03.599437'::TIMESTAMP,'TRUE',12,2,'toba')</v>
+      </c>
+      <c r="K3" t="s">
+        <f>H3&amp;I3&amp;";"</f>
+        <v>16</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -539,32 +549,35 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="str">
-        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;D4&amp;","&amp;E4&amp;")"</f>
-        <v>3,'2017-09-30 09:37:15.278727'::TIMESTAMP,'TRUE',14,2)</v>
-      </c>
-      <c r="J4" t="s">
-        <f>G4&amp;H4&amp;";"</f>
-        <v>18</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="K8" s="2"/>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="str">
+        <f>A4&amp;","&amp;"'"&amp;B4&amp;"'"&amp;"::TIMESTAMP"&amp;","&amp;"'"&amp;C4&amp;"'"&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;"'"&amp;F4&amp;"'"&amp;")"</f>
+        <v>3,'2017-09-30 09:37:15.278727'::TIMESTAMP,'TRUE',14,2,'toba')</v>
+      </c>
+      <c r="K4" t="s">
+        <f>H4&amp;I4&amp;";"</f>
+        <v>17</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="L8" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -601,10 +614,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -643,13 +656,13 @@
         </is>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" t="str">
         <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;"'"&amp;E2&amp;"'"&amp;","&amp;F2&amp;","&amp;G2&amp;")"</f>
@@ -657,10 +670,10 @@
       </c>
       <c r="M2" t="s">
         <f>J2&amp;K2&amp;";"</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -682,13 +695,13 @@
         </is>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" t="str">
         <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;"'"&amp;E3&amp;"'"&amp;","&amp;F3&amp;","&amp;G3&amp;")"</f>
@@ -696,10 +709,10 @@
       </c>
       <c r="M3" t="s">
         <f>J3&amp;K3&amp;";"</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -721,13 +734,13 @@
         </is>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" t="str">
         <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;"'"&amp;E4&amp;"'"&amp;","&amp;F4&amp;","&amp;G4&amp;")"</f>
@@ -735,10 +748,10 @@
       </c>
       <c r="M4" t="s">
         <f>J4&amp;K4&amp;";"</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -768,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" t="str">
         <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;"'"&amp;E5&amp;"'"&amp;","&amp;F5&amp;","&amp;G5&amp;")"</f>
@@ -776,10 +789,10 @@
       </c>
       <c r="M5" t="s">
         <f>J5&amp;K5&amp;";"</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +814,7 @@
   </sheetPr>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="75" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="75">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -829,17 +842,17 @@
         </is>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
@@ -869,13 +882,13 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" t="str">
         <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;H2&amp;","&amp;I2&amp;")"</f>
@@ -883,10 +896,10 @@
       </c>
       <c r="O2" t="s">
         <f>L2&amp;M2&amp;";"</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -909,13 +922,13 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3" t="str">
         <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;H3&amp;","&amp;I3&amp;")"</f>
@@ -923,10 +936,10 @@
       </c>
       <c r="O3" t="s">
         <f>L3&amp;M3&amp;";"</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -949,13 +962,13 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" t="str">
         <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;H4&amp;","&amp;I4&amp;")"</f>
@@ -963,10 +976,10 @@
       </c>
       <c r="O4" t="s">
         <f>L4&amp;M4&amp;";"</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -989,13 +1002,13 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" t="str">
         <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;H5&amp;","&amp;I5&amp;")"</f>
@@ -1003,10 +1016,10 @@
       </c>
       <c r="O5" t="s">
         <f>L5&amp;M5&amp;";"</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1029,13 +1042,13 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" t="str">
         <f>A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;","&amp;H6&amp;","&amp;I6&amp;")"</f>
@@ -1043,10 +1056,10 @@
       </c>
       <c r="O6" t="s">
         <f>L6&amp;M6&amp;";"</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1069,13 +1082,13 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" t="str">
         <f>A7&amp;","&amp;B7&amp;","&amp;C7&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;H7&amp;","&amp;I7&amp;")"</f>
@@ -1083,10 +1096,10 @@
       </c>
       <c r="O7" t="s">
         <f>L7&amp;M7&amp;";"</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>